<commit_message>
Automation of Balancesheet scenarios
</commit_message>
<xml_diff>
--- a/tests/artifact/script/BalanceSheet.xlsx
+++ b/tests/artifact/script/BalanceSheet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Login" sheetId="10" r:id="rId2"/>
-    <sheet name="BalanceSheet" sheetId="12" r:id="rId3"/>
+    <sheet name="BalanceSheet_Scenarios" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="904">
   <si>
     <t>target</t>
   </si>
@@ -2260,7 +2260,7 @@
     <t>execution summary</t>
   </si>
   <si>
-    <t>Invalid login to the Accionconnect website</t>
+    <t>login to the Accionconnect website</t>
   </si>
   <si>
     <t>activity</t>
@@ -2315,10 +2315,10 @@
 password=${password}</t>
   </si>
   <si>
-    <t>Balancesheet Details</t>
-  </si>
-  <si>
-    <t>Go to BalanceSheet page</t>
+    <t>Balancesheet Automation Test Cases</t>
+  </si>
+  <si>
+    <t>Go to BalanceSheet page Redirection</t>
   </si>
   <si>
     <t>click on open organization button</t>
@@ -2354,7 +2354,7 @@
     <t>${org.balancesheet}</t>
   </si>
   <si>
-    <t>Add BalanceSheet</t>
+    <t>Add BalanceSheet to the Organization</t>
   </si>
   <si>
     <t>Click and validate 'BalanceSheet' title</t>
@@ -2775,9 +2775,6 @@
   </si>
   <si>
     <t>click on getdetails button to get the list of all the details</t>
-  </si>
-  <si>
-    <t>Negative TC for Go to BalanceSheet page</t>
   </si>
 </sst>
 </file>
@@ -6851,7 +6848,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -9836,15 +9833,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O134"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="61.75" style="6" customWidth="1"/>
+    <col min="1" max="1" width="52.375" style="6" customWidth="1"/>
     <col min="2" max="2" width="81.375" style="7" customWidth="1"/>
     <col min="3" max="3" width="10" style="8" customWidth="1"/>
     <col min="4" max="4" width="47.3333333333333" style="9" customWidth="1"/>
@@ -11683,1717 +11680,6 @@
       <c r="M69" s="33"/>
       <c r="N69" s="59"/>
       <c r="O69" s="34"/>
-    </row>
-    <row r="70" s="4" customFormat="1" ht="26" customHeight="1" spans="1:15">
-      <c r="A70" s="31" t="s">
-        <v>904</v>
-      </c>
-      <c r="B70" s="32" t="s">
-        <v>752</v>
-      </c>
-      <c r="C70" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D70" s="34" t="s">
-        <v>576</v>
-      </c>
-      <c r="E70" s="35" t="s">
-        <v>753</v>
-      </c>
-      <c r="F70" s="36">
-        <v>1500</v>
-      </c>
-      <c r="G70" s="34"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="34"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="34"/>
-      <c r="L70" s="59"/>
-      <c r="M70" s="33"/>
-      <c r="N70" s="59"/>
-      <c r="O70" s="34"/>
-    </row>
-    <row r="71" s="4" customFormat="1" ht="22" customHeight="1" spans="1:15">
-      <c r="A71" s="31"/>
-      <c r="B71" s="24" t="s">
-        <v>754</v>
-      </c>
-      <c r="C71" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E71" s="35" t="s">
-        <v>755</v>
-      </c>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="34"/>
-      <c r="J71" s="38"/>
-      <c r="K71" s="34"/>
-      <c r="L71" s="59"/>
-      <c r="M71" s="33"/>
-      <c r="N71" s="59"/>
-      <c r="O71" s="34"/>
-    </row>
-    <row r="72" s="4" customFormat="1" ht="22" customHeight="1" spans="1:15">
-      <c r="A72" s="31"/>
-      <c r="B72" s="24" t="s">
-        <v>756</v>
-      </c>
-      <c r="C72" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="34" t="s">
-        <v>540</v>
-      </c>
-      <c r="E72" s="35" t="s">
-        <v>757</v>
-      </c>
-      <c r="F72" s="34"/>
-      <c r="G72" s="34"/>
-      <c r="H72" s="34"/>
-      <c r="I72" s="34"/>
-      <c r="J72" s="38"/>
-      <c r="K72" s="34"/>
-      <c r="L72" s="59"/>
-      <c r="M72" s="33"/>
-      <c r="N72" s="59"/>
-      <c r="O72" s="34"/>
-    </row>
-    <row r="73" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A73" s="31"/>
-      <c r="B73" s="24" t="s">
-        <v>758</v>
-      </c>
-      <c r="C73" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D73" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E73" s="35" t="s">
-        <v>759</v>
-      </c>
-      <c r="F73" s="34"/>
-      <c r="G73" s="34"/>
-      <c r="H73" s="34"/>
-      <c r="I73" s="34"/>
-      <c r="J73" s="38"/>
-      <c r="K73" s="34"/>
-      <c r="L73" s="59"/>
-      <c r="M73" s="33"/>
-      <c r="N73" s="59"/>
-      <c r="O73" s="34"/>
-    </row>
-    <row r="74" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A74" s="31"/>
-      <c r="B74" s="24" t="s">
-        <v>760</v>
-      </c>
-      <c r="C74" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="34" t="s">
-        <v>540</v>
-      </c>
-      <c r="E74" s="37">
-        <v>1000</v>
-      </c>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="38"/>
-      <c r="K74" s="34"/>
-      <c r="L74" s="59"/>
-      <c r="M74" s="33"/>
-      <c r="N74" s="59"/>
-      <c r="O74" s="34"/>
-    </row>
-    <row r="75" s="4" customFormat="1" ht="29" customHeight="1" spans="1:15">
-      <c r="A75" s="31"/>
-      <c r="B75" s="24" t="s">
-        <v>761</v>
-      </c>
-      <c r="C75" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D75" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E75" s="35" t="s">
-        <v>762</v>
-      </c>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="34"/>
-      <c r="L75" s="59"/>
-      <c r="M75" s="33"/>
-      <c r="N75" s="59"/>
-      <c r="O75" s="34"/>
-    </row>
-    <row r="76" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A76" s="23" t="s">
-        <v>763</v>
-      </c>
-      <c r="B76" s="38" t="s">
-        <v>756</v>
-      </c>
-      <c r="C76" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D76" s="34" t="s">
-        <v>714</v>
-      </c>
-      <c r="E76" s="37">
-        <v>2000</v>
-      </c>
-      <c r="F76" s="34"/>
-      <c r="G76" s="34"/>
-      <c r="H76" s="26"/>
-      <c r="I76" s="26"/>
-      <c r="J76" s="24"/>
-      <c r="K76" s="26"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="28"/>
-      <c r="O76" s="26"/>
-    </row>
-    <row r="77" s="5" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A77" s="39"/>
-      <c r="B77" s="24" t="s">
-        <v>764</v>
-      </c>
-      <c r="C77" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D77" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E77" s="35" t="s">
-        <v>765</v>
-      </c>
-      <c r="F77" s="40" t="s">
-        <v>766</v>
-      </c>
-      <c r="G77" s="41"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="42"/>
-      <c r="J77" s="60"/>
-      <c r="K77" s="42"/>
-      <c r="L77" s="61"/>
-      <c r="M77" s="62"/>
-      <c r="N77" s="61"/>
-      <c r="O77" s="42"/>
-    </row>
-    <row r="78" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A78" s="23" t="s">
-        <v>767</v>
-      </c>
-      <c r="B78" s="24" t="s">
-        <v>768</v>
-      </c>
-      <c r="C78" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D78" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E78" s="27" t="s">
-        <v>769</v>
-      </c>
-      <c r="F78" s="26"/>
-      <c r="G78" s="34"/>
-      <c r="H78" s="26"/>
-      <c r="I78" s="26"/>
-      <c r="J78" s="24"/>
-      <c r="K78" s="26"/>
-      <c r="L78" s="28"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="28"/>
-      <c r="O78" s="26"/>
-    </row>
-    <row r="79" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A79" s="23"/>
-      <c r="B79" s="24" t="s">
-        <v>768</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E79" s="43" t="s">
-        <v>770</v>
-      </c>
-      <c r="F79" s="44" t="s">
-        <v>771</v>
-      </c>
-      <c r="G79" s="34"/>
-      <c r="H79" s="26"/>
-      <c r="I79" s="26"/>
-      <c r="J79" s="24"/>
-      <c r="K79" s="26"/>
-      <c r="L79" s="28"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="28"/>
-      <c r="O79" s="26"/>
-    </row>
-    <row r="80" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24" t="s">
-        <v>772</v>
-      </c>
-      <c r="C80" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D80" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E80" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="F80" s="45"/>
-      <c r="G80" s="34"/>
-      <c r="H80" s="26"/>
-      <c r="I80" s="26"/>
-      <c r="J80" s="24"/>
-      <c r="K80" s="26"/>
-      <c r="L80" s="28"/>
-      <c r="M80" s="25"/>
-      <c r="N80" s="28"/>
-      <c r="O80" s="26"/>
-    </row>
-    <row r="81" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A81" s="23"/>
-      <c r="B81" s="24" t="s">
-        <v>774</v>
-      </c>
-      <c r="C81" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D81" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E81" s="27" t="s">
-        <v>775</v>
-      </c>
-      <c r="F81" s="45" t="s">
-        <v>776</v>
-      </c>
-      <c r="G81" s="34"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="26"/>
-      <c r="J81" s="24"/>
-      <c r="K81" s="26"/>
-      <c r="L81" s="28"/>
-      <c r="M81" s="25"/>
-      <c r="N81" s="28"/>
-      <c r="O81" s="26"/>
-    </row>
-    <row r="82" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24" t="s">
-        <v>777</v>
-      </c>
-      <c r="C82" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>778</v>
-      </c>
-      <c r="F82" s="45"/>
-      <c r="G82" s="34"/>
-      <c r="H82" s="26"/>
-      <c r="I82" s="26"/>
-      <c r="J82" s="24"/>
-      <c r="K82" s="26"/>
-      <c r="L82" s="28"/>
-      <c r="M82" s="25"/>
-      <c r="N82" s="28"/>
-      <c r="O82" s="26"/>
-    </row>
-    <row r="83" s="4" customFormat="1" ht="22" customHeight="1" spans="1:10">
-      <c r="A83" s="23"/>
-      <c r="B83" s="24" t="s">
-        <v>779</v>
-      </c>
-      <c r="C83" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D83" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E83" s="43" t="s">
-        <v>780</v>
-      </c>
-      <c r="F83" s="46" t="s">
-        <v>781</v>
-      </c>
-      <c r="G83" s="34"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32"/>
-      <c r="J83" s="32"/>
-    </row>
-    <row r="84" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A84" s="23"/>
-      <c r="B84" s="24" t="s">
-        <v>782</v>
-      </c>
-      <c r="C84" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E84" s="27" t="s">
-        <v>783</v>
-      </c>
-      <c r="F84" s="45"/>
-      <c r="G84" s="34"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="26"/>
-      <c r="J84" s="24"/>
-      <c r="K84" s="26"/>
-      <c r="L84" s="28"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="28"/>
-      <c r="O84" s="26"/>
-    </row>
-    <row r="85" s="4" customFormat="1" ht="22" customHeight="1" spans="1:10">
-      <c r="A85" s="23"/>
-      <c r="B85" s="32" t="s">
-        <v>784</v>
-      </c>
-      <c r="C85" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D85" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E85" s="43" t="s">
-        <v>785</v>
-      </c>
-      <c r="F85" s="32"/>
-      <c r="G85" s="34"/>
-      <c r="H85" s="32"/>
-      <c r="I85" s="32"/>
-      <c r="J85" s="32"/>
-    </row>
-    <row r="86" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A86" s="23"/>
-      <c r="B86" s="24" t="s">
-        <v>786</v>
-      </c>
-      <c r="C86" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D86" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E86" s="27" t="s">
-        <v>787</v>
-      </c>
-      <c r="F86" s="45"/>
-      <c r="G86" s="34"/>
-      <c r="H86" s="26"/>
-      <c r="I86" s="26"/>
-      <c r="J86" s="24"/>
-      <c r="K86" s="26"/>
-      <c r="L86" s="28"/>
-      <c r="M86" s="25"/>
-      <c r="N86" s="28"/>
-      <c r="O86" s="26"/>
-    </row>
-    <row r="87" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A87" s="23"/>
-      <c r="B87" s="24" t="s">
-        <v>788</v>
-      </c>
-      <c r="C87" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>789</v>
-      </c>
-      <c r="F87" s="45"/>
-      <c r="G87" s="34"/>
-      <c r="H87" s="26"/>
-      <c r="I87" s="26"/>
-      <c r="J87" s="24"/>
-      <c r="K87" s="26"/>
-      <c r="L87" s="28"/>
-      <c r="M87" s="25"/>
-      <c r="N87" s="28"/>
-      <c r="O87" s="26"/>
-    </row>
-    <row r="88" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A88" s="31" t="s">
-        <v>790</v>
-      </c>
-      <c r="B88" s="24" t="s">
-        <v>791</v>
-      </c>
-      <c r="C88" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D88" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E88" s="43" t="s">
-        <v>792</v>
-      </c>
-      <c r="F88" s="46" t="s">
-        <v>793</v>
-      </c>
-      <c r="G88" s="34"/>
-      <c r="H88" s="26"/>
-      <c r="I88" s="26"/>
-      <c r="J88" s="24"/>
-      <c r="K88" s="26"/>
-      <c r="L88" s="28"/>
-      <c r="M88" s="25"/>
-      <c r="N88" s="28"/>
-      <c r="O88" s="26"/>
-    </row>
-    <row r="89" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A89" s="23"/>
-      <c r="B89" s="38" t="s">
-        <v>794</v>
-      </c>
-      <c r="C89" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E89" s="35" t="s">
-        <v>795</v>
-      </c>
-      <c r="F89" s="47" t="s">
-        <v>796</v>
-      </c>
-      <c r="G89" s="34"/>
-      <c r="H89" s="26"/>
-      <c r="I89" s="26"/>
-      <c r="J89" s="24"/>
-      <c r="K89" s="26"/>
-      <c r="L89" s="28"/>
-      <c r="M89" s="25"/>
-      <c r="N89" s="28"/>
-      <c r="O89" s="26"/>
-    </row>
-    <row r="90" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A90" s="23"/>
-      <c r="B90" s="38" t="s">
-        <v>797</v>
-      </c>
-      <c r="C90" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E90" s="48" t="s">
-        <v>798</v>
-      </c>
-      <c r="F90" s="47" t="s">
-        <v>799</v>
-      </c>
-      <c r="G90" s="34"/>
-      <c r="H90" s="26"/>
-      <c r="I90" s="26"/>
-      <c r="J90" s="24"/>
-      <c r="K90" s="26"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="25"/>
-      <c r="N90" s="28"/>
-      <c r="O90" s="26"/>
-    </row>
-    <row r="91" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A91" s="31"/>
-      <c r="B91" s="38" t="s">
-        <v>800</v>
-      </c>
-      <c r="C91" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D91" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E91" s="35" t="s">
-        <v>801</v>
-      </c>
-      <c r="F91" s="34" t="s">
-        <v>802</v>
-      </c>
-      <c r="G91" s="34"/>
-      <c r="H91" s="34"/>
-      <c r="I91" s="34"/>
-      <c r="J91" s="38"/>
-      <c r="K91" s="34"/>
-      <c r="L91" s="59"/>
-      <c r="M91" s="33"/>
-      <c r="N91" s="59"/>
-      <c r="O91" s="34"/>
-    </row>
-    <row r="92" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A92" s="31"/>
-      <c r="B92" s="38" t="s">
-        <v>803</v>
-      </c>
-      <c r="C92" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D92" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E92" s="35" t="s">
-        <v>804</v>
-      </c>
-      <c r="F92" s="34" t="s">
-        <v>805</v>
-      </c>
-      <c r="G92" s="34"/>
-      <c r="H92" s="34"/>
-      <c r="I92" s="34"/>
-      <c r="J92" s="38"/>
-      <c r="K92" s="34"/>
-      <c r="L92" s="59"/>
-      <c r="M92" s="33"/>
-      <c r="N92" s="59"/>
-      <c r="O92" s="34"/>
-    </row>
-    <row r="93" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A93" s="31"/>
-      <c r="B93" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C93" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E93" s="35" t="s">
-        <v>807</v>
-      </c>
-      <c r="F93" s="49" t="s">
-        <v>808</v>
-      </c>
-      <c r="G93" s="34"/>
-      <c r="H93" s="34"/>
-      <c r="I93" s="34"/>
-      <c r="J93" s="38"/>
-      <c r="K93" s="34"/>
-      <c r="L93" s="59"/>
-      <c r="M93" s="33"/>
-      <c r="N93" s="59"/>
-      <c r="O93" s="34"/>
-    </row>
-    <row r="94" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A94" s="31"/>
-      <c r="B94" s="38" t="s">
-        <v>809</v>
-      </c>
-      <c r="C94" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="26" t="s">
-        <v>536</v>
-      </c>
-      <c r="E94" s="35" t="s">
-        <v>810</v>
-      </c>
-      <c r="F94" s="49"/>
-      <c r="G94" s="34"/>
-      <c r="H94" s="34"/>
-      <c r="I94" s="34"/>
-      <c r="J94" s="38"/>
-      <c r="K94" s="34"/>
-      <c r="L94" s="59"/>
-      <c r="M94" s="33"/>
-      <c r="N94" s="59"/>
-      <c r="O94" s="34"/>
-    </row>
-    <row r="95" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A95" s="31"/>
-      <c r="B95" s="38" t="s">
-        <v>811</v>
-      </c>
-      <c r="C95" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D95" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E95" s="35" t="s">
-        <v>812</v>
-      </c>
-      <c r="F95" s="49" t="s">
-        <v>810</v>
-      </c>
-      <c r="G95" s="34"/>
-      <c r="H95" s="34"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="38"/>
-      <c r="K95" s="34"/>
-      <c r="L95" s="59"/>
-      <c r="M95" s="33"/>
-      <c r="N95" s="59"/>
-      <c r="O95" s="34"/>
-    </row>
-    <row r="96" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A96" s="31"/>
-      <c r="B96" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C96" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D96" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E96" s="49" t="s">
-        <v>813</v>
-      </c>
-      <c r="F96" s="35" t="s">
-        <v>814</v>
-      </c>
-      <c r="G96" s="50"/>
-      <c r="H96" s="34"/>
-      <c r="I96" s="34"/>
-      <c r="J96" s="38"/>
-      <c r="K96" s="34"/>
-      <c r="L96" s="59"/>
-      <c r="M96" s="33"/>
-      <c r="N96" s="59"/>
-      <c r="O96" s="34"/>
-    </row>
-    <row r="97" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A97" s="31"/>
-      <c r="B97" s="38" t="s">
-        <v>815</v>
-      </c>
-      <c r="C97" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D97" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E97" s="35" t="s">
-        <v>816</v>
-      </c>
-      <c r="F97" s="49" t="s">
-        <v>817</v>
-      </c>
-      <c r="G97" s="34"/>
-      <c r="H97" s="34"/>
-      <c r="I97" s="34"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="34"/>
-      <c r="L97" s="59"/>
-      <c r="M97" s="33"/>
-      <c r="N97" s="59"/>
-      <c r="O97" s="34"/>
-    </row>
-    <row r="98" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A98" s="31"/>
-      <c r="B98" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C98" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D98" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E98" s="49" t="s">
-        <v>818</v>
-      </c>
-      <c r="F98" s="35" t="s">
-        <v>819</v>
-      </c>
-      <c r="G98" s="50"/>
-      <c r="H98" s="34"/>
-      <c r="I98" s="34"/>
-      <c r="J98" s="38"/>
-      <c r="K98" s="34"/>
-      <c r="L98" s="59"/>
-      <c r="M98" s="33"/>
-      <c r="N98" s="59"/>
-      <c r="O98" s="34"/>
-    </row>
-    <row r="99" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A99" s="31"/>
-      <c r="B99" s="38" t="s">
-        <v>815</v>
-      </c>
-      <c r="C99" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E99" s="35" t="s">
-        <v>820</v>
-      </c>
-      <c r="F99" s="49" t="s">
-        <v>819</v>
-      </c>
-      <c r="G99" s="34"/>
-      <c r="H99" s="34"/>
-      <c r="I99" s="34"/>
-      <c r="J99" s="38"/>
-      <c r="K99" s="34"/>
-      <c r="L99" s="59"/>
-      <c r="M99" s="33"/>
-      <c r="N99" s="59"/>
-      <c r="O99" s="34"/>
-    </row>
-    <row r="100" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A100" s="31"/>
-      <c r="B100" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C100" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D100" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E100" s="49" t="s">
-        <v>821</v>
-      </c>
-      <c r="F100" s="35" t="s">
-        <v>822</v>
-      </c>
-      <c r="G100" s="50"/>
-      <c r="H100" s="34"/>
-      <c r="I100" s="34"/>
-      <c r="J100" s="38"/>
-      <c r="K100" s="34"/>
-      <c r="L100" s="59"/>
-      <c r="M100" s="33"/>
-      <c r="N100" s="59"/>
-      <c r="O100" s="34"/>
-    </row>
-    <row r="101" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A101" s="31"/>
-      <c r="B101" s="38" t="s">
-        <v>823</v>
-      </c>
-      <c r="C101" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D101" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E101" s="35" t="s">
-        <v>824</v>
-      </c>
-      <c r="F101" s="49" t="s">
-        <v>822</v>
-      </c>
-      <c r="G101" s="34"/>
-      <c r="H101" s="34"/>
-      <c r="I101" s="34"/>
-      <c r="J101" s="38"/>
-      <c r="K101" s="34"/>
-      <c r="L101" s="59"/>
-      <c r="M101" s="33"/>
-      <c r="N101" s="59"/>
-      <c r="O101" s="34"/>
-    </row>
-    <row r="102" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A102" s="31"/>
-      <c r="B102" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C102" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D102" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E102" s="49" t="s">
-        <v>825</v>
-      </c>
-      <c r="F102" s="35" t="s">
-        <v>826</v>
-      </c>
-      <c r="G102" s="50"/>
-      <c r="H102" s="34"/>
-      <c r="I102" s="34"/>
-      <c r="J102" s="38"/>
-      <c r="K102" s="34"/>
-      <c r="L102" s="59"/>
-      <c r="M102" s="33"/>
-      <c r="N102" s="59"/>
-      <c r="O102" s="34"/>
-    </row>
-    <row r="103" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A103" s="31"/>
-      <c r="B103" s="38" t="s">
-        <v>827</v>
-      </c>
-      <c r="C103" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D103" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E103" s="35" t="s">
-        <v>828</v>
-      </c>
-      <c r="F103" s="49" t="s">
-        <v>826</v>
-      </c>
-      <c r="G103" s="34"/>
-      <c r="H103" s="34"/>
-      <c r="I103" s="34"/>
-      <c r="J103" s="38"/>
-      <c r="K103" s="34"/>
-      <c r="L103" s="59"/>
-      <c r="M103" s="33"/>
-      <c r="N103" s="59"/>
-      <c r="O103" s="34"/>
-    </row>
-    <row r="104" s="1" customFormat="1" ht="15" spans="1:15">
-      <c r="A104" s="31" t="s">
-        <v>829</v>
-      </c>
-      <c r="B104" s="38" t="s">
-        <v>830</v>
-      </c>
-      <c r="C104" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D104" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E104" s="35" t="s">
-        <v>831</v>
-      </c>
-      <c r="F104" s="34" t="s">
-        <v>832</v>
-      </c>
-      <c r="G104" s="34"/>
-      <c r="H104" s="34"/>
-      <c r="I104" s="34"/>
-      <c r="J104" s="38"/>
-      <c r="K104" s="34"/>
-      <c r="L104" s="59"/>
-      <c r="M104" s="33"/>
-      <c r="N104" s="59"/>
-      <c r="O104" s="34"/>
-    </row>
-    <row r="105" s="1" customFormat="1" ht="15" spans="1:15">
-      <c r="A105" s="31"/>
-      <c r="B105" s="38" t="s">
-        <v>833</v>
-      </c>
-      <c r="C105" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D105" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E105" s="27" t="s">
-        <v>834</v>
-      </c>
-      <c r="F105" s="26" t="s">
-        <v>835</v>
-      </c>
-      <c r="G105" s="34"/>
-      <c r="H105" s="34"/>
-      <c r="I105" s="34"/>
-      <c r="J105" s="38"/>
-      <c r="K105" s="34"/>
-      <c r="L105" s="59"/>
-      <c r="M105" s="33"/>
-      <c r="N105" s="59"/>
-      <c r="O105" s="34"/>
-    </row>
-    <row r="106" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A106" s="31"/>
-      <c r="B106" s="38" t="s">
-        <v>836</v>
-      </c>
-      <c r="C106" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D106" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E106" s="35" t="s">
-        <v>837</v>
-      </c>
-      <c r="F106" s="26" t="s">
-        <v>838</v>
-      </c>
-      <c r="G106" s="34"/>
-      <c r="H106" s="34"/>
-      <c r="I106" s="34"/>
-      <c r="J106" s="38"/>
-      <c r="K106" s="34"/>
-      <c r="L106" s="59"/>
-      <c r="M106" s="33"/>
-      <c r="N106" s="59"/>
-      <c r="O106" s="34"/>
-    </row>
-    <row r="107" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A107" s="31"/>
-      <c r="B107" s="38" t="s">
-        <v>839</v>
-      </c>
-      <c r="C107" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D107" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E107" s="27" t="s">
-        <v>840</v>
-      </c>
-      <c r="F107" s="26" t="s">
-        <v>841</v>
-      </c>
-      <c r="G107" s="34"/>
-      <c r="H107" s="34"/>
-      <c r="I107" s="34"/>
-      <c r="J107" s="38"/>
-      <c r="K107" s="34"/>
-      <c r="L107" s="59"/>
-      <c r="M107" s="33"/>
-      <c r="N107" s="59"/>
-      <c r="O107" s="34"/>
-    </row>
-    <row r="108" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A108" s="31"/>
-      <c r="B108" s="38" t="s">
-        <v>842</v>
-      </c>
-      <c r="C108" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D108" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E108" s="35" t="s">
-        <v>843</v>
-      </c>
-      <c r="F108" s="26" t="s">
-        <v>844</v>
-      </c>
-      <c r="G108" s="34"/>
-      <c r="H108" s="34"/>
-      <c r="I108" s="34"/>
-      <c r="J108" s="38"/>
-      <c r="K108" s="34"/>
-      <c r="L108" s="59"/>
-      <c r="M108" s="33"/>
-      <c r="N108" s="59"/>
-      <c r="O108" s="34"/>
-    </row>
-    <row r="109" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A109" s="23"/>
-      <c r="B109" s="38" t="s">
-        <v>845</v>
-      </c>
-      <c r="C109" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D109" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E109" s="51" t="s">
-        <v>846</v>
-      </c>
-      <c r="F109" s="26" t="s">
-        <v>847</v>
-      </c>
-      <c r="G109" s="34"/>
-      <c r="H109" s="26"/>
-      <c r="I109" s="26"/>
-      <c r="J109" s="24"/>
-      <c r="K109" s="26"/>
-      <c r="L109" s="28"/>
-      <c r="M109" s="25"/>
-      <c r="N109" s="28"/>
-      <c r="O109" s="26"/>
-    </row>
-    <row r="110" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A110" s="23"/>
-      <c r="B110" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C110" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D110" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E110" s="49" t="s">
-        <v>848</v>
-      </c>
-      <c r="F110" s="35" t="s">
-        <v>849</v>
-      </c>
-      <c r="G110" s="47"/>
-      <c r="H110" s="26"/>
-      <c r="I110" s="26"/>
-      <c r="J110" s="24"/>
-      <c r="K110" s="26"/>
-      <c r="L110" s="28"/>
-      <c r="M110" s="25"/>
-      <c r="N110" s="28"/>
-      <c r="O110" s="26"/>
-    </row>
-    <row r="111" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A111" s="31"/>
-      <c r="B111" s="38" t="s">
-        <v>850</v>
-      </c>
-      <c r="C111" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D111" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E111" s="35" t="s">
-        <v>851</v>
-      </c>
-      <c r="F111" s="34" t="s">
-        <v>852</v>
-      </c>
-      <c r="G111" s="34"/>
-      <c r="H111" s="34"/>
-      <c r="I111" s="34"/>
-      <c r="J111" s="38"/>
-      <c r="K111" s="34"/>
-      <c r="L111" s="59"/>
-      <c r="M111" s="33"/>
-      <c r="N111" s="59"/>
-      <c r="O111" s="34"/>
-    </row>
-    <row r="112" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A112" s="23"/>
-      <c r="B112" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C112" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D112" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E112" s="49" t="s">
-        <v>853</v>
-      </c>
-      <c r="F112" s="35" t="s">
-        <v>854</v>
-      </c>
-      <c r="G112" s="47"/>
-      <c r="H112" s="26"/>
-      <c r="I112" s="26"/>
-      <c r="J112" s="24"/>
-      <c r="K112" s="26"/>
-      <c r="L112" s="28"/>
-      <c r="M112" s="25"/>
-      <c r="N112" s="28"/>
-      <c r="O112" s="26"/>
-    </row>
-    <row r="113" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A113" s="31"/>
-      <c r="B113" s="38" t="s">
-        <v>855</v>
-      </c>
-      <c r="C113" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D113" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E113" s="35" t="s">
-        <v>856</v>
-      </c>
-      <c r="F113" s="49" t="s">
-        <v>857</v>
-      </c>
-      <c r="G113" s="34"/>
-      <c r="H113" s="34"/>
-      <c r="I113" s="34"/>
-      <c r="J113" s="38"/>
-      <c r="K113" s="34"/>
-      <c r="L113" s="59"/>
-      <c r="M113" s="33"/>
-      <c r="N113" s="59"/>
-      <c r="O113" s="34"/>
-    </row>
-    <row r="114" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A114" s="31"/>
-      <c r="B114" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C114" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D114" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E114" s="34" t="s">
-        <v>858</v>
-      </c>
-      <c r="F114" s="35" t="s">
-        <v>859</v>
-      </c>
-      <c r="G114" s="50"/>
-      <c r="H114" s="34"/>
-      <c r="I114" s="34"/>
-      <c r="J114" s="38"/>
-      <c r="K114" s="34"/>
-      <c r="L114" s="59"/>
-      <c r="M114" s="33"/>
-      <c r="N114" s="59"/>
-      <c r="O114" s="34"/>
-    </row>
-    <row r="115" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A115" s="31"/>
-      <c r="B115" s="38" t="s">
-        <v>860</v>
-      </c>
-      <c r="C115" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D115" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E115" s="35" t="s">
-        <v>861</v>
-      </c>
-      <c r="F115" s="34" t="s">
-        <v>862</v>
-      </c>
-      <c r="G115" s="34"/>
-      <c r="H115" s="34"/>
-      <c r="I115" s="34"/>
-      <c r="J115" s="38"/>
-      <c r="K115" s="34"/>
-      <c r="L115" s="59"/>
-      <c r="M115" s="33"/>
-      <c r="N115" s="59"/>
-      <c r="O115" s="34"/>
-    </row>
-    <row r="116" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A116" s="31"/>
-      <c r="B116" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C116" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D116" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E116" s="34" t="s">
-        <v>863</v>
-      </c>
-      <c r="F116" s="35" t="s">
-        <v>864</v>
-      </c>
-      <c r="G116" s="50"/>
-      <c r="H116" s="34"/>
-      <c r="I116" s="34"/>
-      <c r="J116" s="38"/>
-      <c r="K116" s="34"/>
-      <c r="L116" s="59"/>
-      <c r="M116" s="33"/>
-      <c r="N116" s="59"/>
-      <c r="O116" s="34"/>
-    </row>
-    <row r="117" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A117" s="31"/>
-      <c r="B117" s="38" t="s">
-        <v>865</v>
-      </c>
-      <c r="C117" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D117" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E117" s="35" t="s">
-        <v>866</v>
-      </c>
-      <c r="F117" s="34" t="s">
-        <v>867</v>
-      </c>
-      <c r="G117" s="34"/>
-      <c r="H117" s="34"/>
-      <c r="I117" s="34"/>
-      <c r="J117" s="38"/>
-      <c r="K117" s="34"/>
-      <c r="L117" s="59"/>
-      <c r="M117" s="33"/>
-      <c r="N117" s="59"/>
-      <c r="O117" s="34"/>
-    </row>
-    <row r="118" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A118" s="31"/>
-      <c r="B118" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C118" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D118" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E118" s="34" t="s">
-        <v>868</v>
-      </c>
-      <c r="F118" s="35" t="s">
-        <v>869</v>
-      </c>
-      <c r="G118" s="50"/>
-      <c r="H118" s="34"/>
-      <c r="I118" s="34"/>
-      <c r="J118" s="38"/>
-      <c r="K118" s="34"/>
-      <c r="L118" s="59"/>
-      <c r="M118" s="33"/>
-      <c r="N118" s="59"/>
-      <c r="O118" s="34"/>
-    </row>
-    <row r="119" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A119" s="31"/>
-      <c r="B119" s="38" t="s">
-        <v>870</v>
-      </c>
-      <c r="C119" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D119" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E119" s="35" t="s">
-        <v>871</v>
-      </c>
-      <c r="F119" s="34" t="s">
-        <v>872</v>
-      </c>
-      <c r="G119" s="34"/>
-      <c r="H119" s="34"/>
-      <c r="I119" s="34"/>
-      <c r="J119" s="38"/>
-      <c r="K119" s="34"/>
-      <c r="L119" s="59"/>
-      <c r="M119" s="33"/>
-      <c r="N119" s="59"/>
-      <c r="O119" s="34"/>
-    </row>
-    <row r="120" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A120" s="31"/>
-      <c r="B120" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C120" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D120" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E120" s="34" t="s">
-        <v>873</v>
-      </c>
-      <c r="F120" s="35" t="s">
-        <v>874</v>
-      </c>
-      <c r="G120" s="50"/>
-      <c r="H120" s="34"/>
-      <c r="I120" s="34"/>
-      <c r="J120" s="38"/>
-      <c r="K120" s="34"/>
-      <c r="L120" s="59"/>
-      <c r="M120" s="33"/>
-      <c r="N120" s="59"/>
-      <c r="O120" s="34"/>
-    </row>
-    <row r="121" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A121" s="31"/>
-      <c r="B121" s="38" t="s">
-        <v>875</v>
-      </c>
-      <c r="C121" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D121" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E121" s="35" t="s">
-        <v>876</v>
-      </c>
-      <c r="F121" s="34" t="s">
-        <v>877</v>
-      </c>
-      <c r="G121" s="34"/>
-      <c r="H121" s="34"/>
-      <c r="I121" s="34"/>
-      <c r="J121" s="38"/>
-      <c r="K121" s="34"/>
-      <c r="L121" s="59"/>
-      <c r="M121" s="33"/>
-      <c r="N121" s="59"/>
-      <c r="O121" s="34"/>
-    </row>
-    <row r="122" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A122" s="31"/>
-      <c r="B122" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C122" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D122" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E122" s="34" t="s">
-        <v>878</v>
-      </c>
-      <c r="F122" s="35" t="s">
-        <v>879</v>
-      </c>
-      <c r="G122" s="50"/>
-      <c r="H122" s="34"/>
-      <c r="I122" s="34"/>
-      <c r="J122" s="38"/>
-      <c r="K122" s="34"/>
-      <c r="L122" s="59"/>
-      <c r="M122" s="33"/>
-      <c r="N122" s="59"/>
-      <c r="O122" s="34"/>
-    </row>
-    <row r="123" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A123" s="31"/>
-      <c r="B123" s="38" t="s">
-        <v>880</v>
-      </c>
-      <c r="C123" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D123" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E123" s="35" t="s">
-        <v>881</v>
-      </c>
-      <c r="F123" s="34" t="s">
-        <v>882</v>
-      </c>
-      <c r="G123" s="34"/>
-      <c r="H123" s="34"/>
-      <c r="I123" s="34"/>
-      <c r="J123" s="38"/>
-      <c r="K123" s="34"/>
-      <c r="L123" s="59"/>
-      <c r="M123" s="33"/>
-      <c r="N123" s="59"/>
-      <c r="O123" s="34"/>
-    </row>
-    <row r="124" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A124" s="31"/>
-      <c r="B124" s="38" t="s">
-        <v>806</v>
-      </c>
-      <c r="C124" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D124" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="E124" s="34" t="s">
-        <v>883</v>
-      </c>
-      <c r="F124" s="35" t="s">
-        <v>884</v>
-      </c>
-      <c r="G124" s="50"/>
-      <c r="H124" s="34"/>
-      <c r="I124" s="34"/>
-      <c r="J124" s="38"/>
-      <c r="K124" s="34"/>
-      <c r="L124" s="59"/>
-      <c r="M124" s="33"/>
-      <c r="N124" s="59"/>
-      <c r="O124" s="34"/>
-    </row>
-    <row r="125" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A125" s="31"/>
-      <c r="B125" s="38" t="s">
-        <v>885</v>
-      </c>
-      <c r="C125" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D125" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="E125" s="35" t="s">
-        <v>886</v>
-      </c>
-      <c r="F125" s="34" t="s">
-        <v>887</v>
-      </c>
-      <c r="G125" s="34"/>
-      <c r="H125" s="34"/>
-      <c r="I125" s="34"/>
-      <c r="J125" s="38"/>
-      <c r="K125" s="34"/>
-      <c r="L125" s="59"/>
-      <c r="M125" s="33"/>
-      <c r="N125" s="59"/>
-      <c r="O125" s="34"/>
-    </row>
-    <row r="126" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A126" s="31"/>
-      <c r="B126" s="38" t="s">
-        <v>888</v>
-      </c>
-      <c r="C126" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D126" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E126" s="35" t="s">
-        <v>889</v>
-      </c>
-      <c r="F126" s="34"/>
-      <c r="G126" s="34"/>
-      <c r="H126" s="34"/>
-      <c r="I126" s="34"/>
-      <c r="J126" s="38"/>
-      <c r="K126" s="34"/>
-      <c r="L126" s="59"/>
-      <c r="M126" s="33"/>
-      <c r="N126" s="59"/>
-      <c r="O126" s="34"/>
-    </row>
-    <row r="127" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A127" s="31"/>
-      <c r="B127" s="38" t="s">
-        <v>890</v>
-      </c>
-      <c r="C127" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D127" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E127" s="35" t="s">
-        <v>891</v>
-      </c>
-      <c r="F127" s="50"/>
-      <c r="G127" s="34"/>
-      <c r="H127" s="34"/>
-      <c r="I127" s="34"/>
-      <c r="J127" s="38"/>
-      <c r="K127" s="34"/>
-      <c r="L127" s="59"/>
-      <c r="M127" s="33"/>
-      <c r="N127" s="59"/>
-      <c r="O127" s="34"/>
-    </row>
-    <row r="128" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A128" s="31"/>
-      <c r="B128" s="38" t="s">
-        <v>892</v>
-      </c>
-      <c r="C128" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D128" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E128" s="35" t="s">
-        <v>893</v>
-      </c>
-      <c r="F128" s="50"/>
-      <c r="G128" s="34"/>
-      <c r="H128" s="34"/>
-      <c r="I128" s="34"/>
-      <c r="J128" s="38"/>
-      <c r="K128" s="34"/>
-      <c r="L128" s="59"/>
-      <c r="M128" s="33"/>
-      <c r="N128" s="59"/>
-      <c r="O128" s="34"/>
-    </row>
-    <row r="129" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A129" s="31"/>
-      <c r="B129" s="38" t="s">
-        <v>894</v>
-      </c>
-      <c r="C129" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D129" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E129" s="27" t="s">
-        <v>895</v>
-      </c>
-      <c r="F129" s="45"/>
-      <c r="G129" s="34"/>
-      <c r="H129" s="34"/>
-      <c r="I129" s="34"/>
-      <c r="J129" s="38"/>
-      <c r="K129" s="34"/>
-      <c r="L129" s="59"/>
-      <c r="M129" s="33"/>
-      <c r="N129" s="59"/>
-      <c r="O129" s="34"/>
-    </row>
-    <row r="130" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A130" s="31" t="s">
-        <v>896</v>
-      </c>
-      <c r="B130" s="24" t="s">
-        <v>897</v>
-      </c>
-      <c r="C130" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D130" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="E130" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="F130" s="45"/>
-      <c r="G130" s="34"/>
-      <c r="H130" s="34"/>
-      <c r="I130" s="34"/>
-      <c r="J130" s="38"/>
-      <c r="K130" s="34"/>
-      <c r="L130" s="59"/>
-      <c r="M130" s="33"/>
-      <c r="N130" s="59"/>
-      <c r="O130" s="34"/>
-    </row>
-    <row r="131" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A131" s="31"/>
-      <c r="B131" s="24" t="s">
-        <v>898</v>
-      </c>
-      <c r="C131" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D131" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="E131" s="63" t="s">
-        <v>899</v>
-      </c>
-      <c r="F131" s="45"/>
-      <c r="G131" s="34"/>
-      <c r="H131" s="34"/>
-      <c r="I131" s="34"/>
-      <c r="J131" s="38"/>
-      <c r="K131" s="34"/>
-      <c r="L131" s="59"/>
-      <c r="M131" s="33"/>
-      <c r="N131" s="59"/>
-      <c r="O131" s="34"/>
-    </row>
-    <row r="132" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A132" s="31"/>
-      <c r="B132" s="24" t="s">
-        <v>900</v>
-      </c>
-      <c r="C132" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D132" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="E132" s="27" t="s">
-        <v>778</v>
-      </c>
-      <c r="F132" s="26"/>
-      <c r="G132" s="34"/>
-      <c r="H132" s="34"/>
-      <c r="I132" s="34"/>
-      <c r="J132" s="38"/>
-      <c r="K132" s="34"/>
-      <c r="L132" s="59"/>
-      <c r="M132" s="33"/>
-      <c r="N132" s="59"/>
-      <c r="O132" s="34"/>
-    </row>
-    <row r="133" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A133" s="31"/>
-      <c r="B133" s="24" t="s">
-        <v>901</v>
-      </c>
-      <c r="C133" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D133" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="E133" s="43" t="s">
-        <v>902</v>
-      </c>
-      <c r="F133" s="26"/>
-      <c r="G133" s="34"/>
-      <c r="H133" s="34"/>
-      <c r="I133" s="34"/>
-      <c r="J133" s="38"/>
-      <c r="K133" s="34"/>
-      <c r="L133" s="59"/>
-      <c r="M133" s="33"/>
-      <c r="N133" s="59"/>
-      <c r="O133" s="34"/>
-    </row>
-    <row r="134" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A134" s="31"/>
-      <c r="B134" s="24" t="s">
-        <v>903</v>
-      </c>
-      <c r="C134" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D134" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="E134" s="43" t="s">
-        <v>780</v>
-      </c>
-      <c r="F134" s="26"/>
-      <c r="G134" s="34"/>
-      <c r="H134" s="34"/>
-      <c r="I134" s="34"/>
-      <c r="J134" s="38"/>
-      <c r="K134" s="34"/>
-      <c r="L134" s="59"/>
-      <c r="M134" s="33"/>
-      <c r="N134" s="59"/>
-      <c r="O134" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13457,50 +11743,6 @@
       <formula>LEFT(N47,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
-    <cfRule type="beginsWith" dxfId="2" priority="21" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N82,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N82,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="19" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N82,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N84">
-    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N84,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N84,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N84,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N90">
-    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N90,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N90,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N90,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N112">
-    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N112,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N112,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N112,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N3:N4">
     <cfRule type="beginsWith" dxfId="2" priority="90" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N3,LEN("PASS"))="PASS"</formula>
@@ -13556,50 +11798,6 @@
       <formula>LEFT(N21,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N70:N75">
-    <cfRule type="beginsWith" dxfId="2" priority="27" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N70,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="26" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N70,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="25" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N70,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N76:N77">
-    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N76,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N76,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="22" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N76,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N78:N81">
-    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N78,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N78,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N78,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N86:N89">
-    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N86,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N86,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N86,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N26:N43 N61:N69">
     <cfRule type="beginsWith" dxfId="0" priority="91" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N26,LEN("WARN"))="WARN"</formula>
@@ -13622,33 +11820,11 @@
       <formula>LEFT(N44,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N91:N108 N126:N134">
-    <cfRule type="beginsWith" dxfId="2" priority="30" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N91,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="29" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N91,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="28" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N91,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N109:N111 N113:N125">
-    <cfRule type="beginsWith" dxfId="2" priority="15" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N109,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N109,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="13" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N109,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C18 C19 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C69 C70 C71 C72 C73 C74 C75 C76 C77 C83 C84 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C122 C123 C124 C125 C134 C13:C14 C15:C17 C20:C26 C39:C43 C61:C64 C65:C68 C78:C79 C80:C82 C85:C91 C104:C108 C126:C129 C130:C133">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C18 C19 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C69 C13:C14 C15:C17 C20:C26 C39:C43 C61:C64 C65:C68">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D122 D123 D124 D125 D134 D20:D22 D23:D27 D38:D43 D61:D64 D65:D68 D85:D87 D88:D92 D103:D108 D126:D129 D130:D133">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D69 D20:D22 D23:D27 D38:D43 D61:D64 D65:D68">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>